<commit_message>
Add check true in sheet
</commit_message>
<xml_diff>
--- a/Infor.xlsx
+++ b/Infor.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="31.21875" defaultRowHeight="15.75" customHeight="1"/>
@@ -369,11 +369,7 @@
           <t>Email</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Năm sinh</t>
-        </is>
-      </c>
+      <c r="C1" s="1" t="n"/>
       <c r="X1" t="inlineStr">
         <is>
           <t>Da gui Email</t>
@@ -391,8 +387,8 @@
           <t>duythong020703@gmail.com</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>2003</v>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -406,8 +402,8 @@
           <t>asasin1234434545@gmail.com</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>2004</v>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -417,9 +413,7 @@
         </is>
       </c>
       <c r="B4" s="3" t="n"/>
-      <c r="C4" s="2" t="n">
-        <v>2004</v>
-      </c>
+      <c r="C4" s="2" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>